<commit_message>
create the RTM and modify the CST-reqs
</commit_message>
<xml_diff>
--- a/Requirement/REQ_Customer_Reqs.xlsx
+++ b/Requirement/REQ_Customer_Reqs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dena\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maya Kind\Desktop\QA\Internal-Banking-System\Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF775EDA-AC45-48D0-A114-6C0D2714CB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51B1FEE-8FB1-4BE2-B64D-DA881919B9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="الورقة1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve"> Project Internet Banking System </t>
   </si>
@@ -39,11 +39,6 @@
     <t>User Categoties</t>
   </si>
   <si>
-    <t xml:space="preserve">
-The client should have direct access to his/her different accounts where he can view the histoty of previous transactions 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">The client should have the ability to perform transactions between different accounts </t>
   </si>
   <si>
@@ -83,13 +78,36 @@
     <t xml:space="preserve">This web portal will serve as an interface for all the banking services where the client can easily access his account/s, 
 perform inter account transactions and to inquire about the previous transactions
 </t>
+  </si>
+  <si>
+    <t>CST_REQ_05</t>
+  </si>
+  <si>
+    <t>the admin should create and edit clients information and their accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The client should have direct access to his/her different accounts 
+</t>
+  </si>
+  <si>
+    <t>CST_REQ_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the client can view the histoty of previous transactions </t>
+  </si>
+  <si>
+    <t>CST_REQ_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web_bases System </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,6 +166,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -188,6 +212,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -195,53 +243,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -479,7 +497,7 @@
   <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -492,11 +510,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -526,90 +544,108 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>10</v>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>7</v>
+      <c r="E3" s="15" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="14"/>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="14"/>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="15"/>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
+      <c r="B7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="B9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="8"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="10"/>
+      <c r="B15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -618,14 +654,15 @@
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="A3:A7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>24</formula>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>67</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>67</formula>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>24</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update RTM to contain User transaction feature
</commit_message>
<xml_diff>
--- a/Requirement/REQ_Customer_Reqs.xlsx
+++ b/Requirement/REQ_Customer_Reqs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maya Kind\Desktop\QA\Internal-Banking-System\Requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51B1FEE-8FB1-4BE2-B64D-DA881919B9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC5F08D-0032-4DC1-8770-CAB7BE4826E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve"> Project Internet Banking System </t>
   </si>
@@ -86,21 +86,15 @@
     <t>the admin should create and edit clients information and their accounts</t>
   </si>
   <si>
+    <t>CST_REQ_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web_bases System </t>
+  </si>
+  <si>
     <t xml:space="preserve">
-The client should have direct access to his/her different accounts 
+The client should have direct access to his/her different accounts and  can view the histoty of previous transactions 
 </t>
-  </si>
-  <si>
-    <t>CST_REQ_06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the client can view the histoty of previous transactions </t>
-  </si>
-  <si>
-    <t>CST_REQ_07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">web_bases System </t>
   </si>
 </sst>
 </file>
@@ -119,18 +113,21 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,6 +233,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -251,10 +252,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +491,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -510,11 +507,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -558,7 +555,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -567,92 +564,83 @@
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+        <v>21</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>21</v>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>18</v>
-      </c>
+      <c r="D8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A3:A6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A3">

</xml_diff>